<commit_message>
Tax Checker Final v1.00
</commit_message>
<xml_diff>
--- a/Documents/Tax Checker.xlsx
+++ b/Documents/Tax Checker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\My Files\My-WorkFiles-Backup\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0630E60-F955-45B0-BC43-AF0C400C0D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B6E20D-9601-4EC5-8889-0BC2DA870314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{47E34C20-F3B6-4417-B647-E842E10E84EB}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="134">
   <si>
     <t>frecno</t>
   </si>
@@ -334,12 +334,6 @@
     <t>total_discount</t>
   </si>
   <si>
-    <t>P00091765</t>
-  </si>
-  <si>
-    <t>P7622300501525</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -451,16 +445,31 @@
     <t>fextprice</t>
   </si>
   <si>
-    <t>P00091769</t>
+    <t>CHOICE1</t>
   </si>
   <si>
-    <t>P00132666</t>
+    <t>MLIK99</t>
   </si>
   <si>
-    <t>P00107029</t>
+    <t>CHOICE49</t>
   </si>
   <si>
-    <t>MG762398</t>
+    <t>COMPLIMENTARY</t>
+  </si>
+  <si>
+    <t>FREE1</t>
+  </si>
+  <si>
+    <t>MLIK32</t>
+  </si>
+  <si>
+    <t>MLIK27</t>
+  </si>
+  <si>
+    <t>MLIK75</t>
+  </si>
+  <si>
+    <t>total SC discount</t>
   </si>
 </sst>
 </file>
@@ -926,24 +935,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE4F2DD-03B4-4EB2-B799-B7EBE31253DA}">
   <dimension ref="A1:AR134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V6" sqref="V6"/>
+      <selection pane="bottomLeft" activeCell="AN34" sqref="AN34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="6" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" style="22" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" style="22" customWidth="1"/>
+    <col min="10" max="17" width="20.7109375" customWidth="1"/>
     <col min="18" max="18" width="1.7109375" style="4" customWidth="1"/>
     <col min="19" max="19" width="11.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="1.7109375" style="4" customWidth="1"/>
@@ -1016,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>2</v>
@@ -1045,10 +1051,8 @@
       <c r="M1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" s="14" t="s">
+      <c r="N1" s="13"/>
+      <c r="O1" s="13" t="s">
         <v>5</v>
       </c>
       <c r="P1" s="13" t="s">
@@ -1112,51 +1116,48 @@
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>311113</v>
+        <v>35710</v>
       </c>
       <c r="C2" t="s">
         <v>128</v>
       </c>
       <c r="D2" s="2">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>54</v>
-      </c>
-      <c r="P2" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="22">
+      <c r="Q2">
         <v>0</v>
       </c>
       <c r="S2" s="8" t="str">
@@ -1166,7 +1167,10 @@
       </c>
       <c r="U2" s="33">
         <f>IF(
-            OR(P2=0, P2=1),
+            AND(
+                OR(P2=0, P2=1),
+                O2&lt;&gt;0
+            ),
             IF(G2&gt;0,
                 Q2,
                 IF(
@@ -1188,7 +1192,10 @@
       </c>
       <c r="V2" s="33">
         <f>IF(
-            OR(P2=0, P2=1),
+            AND(
+                OR(P2=0, P2=1),
+                O2&lt;&gt;0
+            ),
             IF(
                 OR(G2&gt;0, H2&gt;0),
                 D2 * E2 - IF(G2&gt;0, Q2, D2 * E2 * H2 / 100),
@@ -1219,9 +1226,9 @@
             ),
             0
         )</f>
-        <v>54</v>
-      </c>
-      <c r="X2" s="1" cm="1">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1" t="str" cm="1">
         <f t="array" ref="X2">IF(
         AND(
             F2=0,
@@ -1233,7 +1240,7 @@
             ROUND((D2 * E2 * PRODUCT(1 - H2:H2 / 100, 1 - L2:L2 / 100, 1 - N2:N2 / 100)), 2)
         ),
     "")</f>
-        <v>54</v>
+        <v/>
       </c>
       <c r="Y2" s="1" t="str" cm="1">
         <f t="array" ref="Y2">IF(
@@ -1320,33 +1327,33 @@
             / 1.12 + AK18
         )
     ), 4)</f>
-        <v>0</v>
+        <v>802.67859999999996</v>
       </c>
       <c r="AP2" s="6">
         <f>AK24
     / AE3
     * (AE3 - AE6 -  AE9 - AE12 - AE15 - AE18 - AE21)
     - (AK3*(AG3/100))</f>
-        <v>276</v>
+        <v>899</v>
       </c>
       <c r="AQ2" s="7">
         <f>AP2 / 1.12 * 0.12</f>
-        <v>29.571428571428569</v>
+        <v>96.321428571428555</v>
       </c>
       <c r="AR2" s="18"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>311113</v>
+        <v>35710</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="D3" s="2">
-        <v>11.5</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1372,16 +1379,13 @@
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>23</v>
-      </c>
-      <c r="P3" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="22">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>0</v>
       </c>
       <c r="S3" s="8" t="str">
@@ -1391,7 +1395,10 @@
       </c>
       <c r="U3" s="33">
         <f t="shared" ref="U3:U66" si="1">IF(
-            OR(P3=0, P3=1),
+            AND(
+                OR(P3=0, P3=1),
+                O3&lt;&gt;0
+            ),
             IF(G3&gt;0,
                 Q3,
                 IF(
@@ -1413,7 +1420,10 @@
       </c>
       <c r="V3" s="33">
         <f t="shared" ref="V3:V66" si="2">IF(
-            OR(P3=0, P3=1),
+            AND(
+                OR(P3=0, P3=1),
+                O3&lt;&gt;0
+            ),
             IF(
                 OR(G3&gt;0, H3&gt;0),
                 D3 * E3 - IF(G3&gt;0, Q3, D3 * E3 * H3 / 100),
@@ -1444,9 +1454,9 @@
             ),
             0
         )</f>
-        <v>23</v>
-      </c>
-      <c r="X3" s="1" cm="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1" t="str" cm="1">
         <f t="array" ref="X3">IF(
         AND(
             F3=0,
@@ -1458,7 +1468,7 @@
             ROUND((D3 * E3 * PRODUCT(1 - H3:H3 / 100, 1 - L3:L3 / 100, 1 - N3:N3 / 100)), 2)
         ),
     "")</f>
-        <v>23</v>
+        <v/>
       </c>
       <c r="Y3" s="1" t="str" cm="1">
         <f t="array" ref="Y3">IF(
@@ -1517,14 +1527,14 @@
         <v/>
       </c>
       <c r="AE3" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG3" s="12">
         <v>0</v>
       </c>
       <c r="AK3" s="5">
         <f>SUM(V:V)</f>
-        <v>276</v>
+        <v>1798</v>
       </c>
       <c r="AL3" s="18"/>
       <c r="AM3" s="18"/>
@@ -1536,13 +1546,13 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>311113</v>
+        <v>35710</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D4" s="2">
-        <v>10</v>
+        <v>488</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1571,16 +1581,13 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2">
-        <v>10</v>
-      </c>
-      <c r="P4" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="22">
+      <c r="O4">
+        <v>488</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <v>0</v>
       </c>
       <c r="S4" s="8" t="str">
@@ -1593,7 +1600,7 @@
       </c>
       <c r="V4" s="33">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>488</v>
       </c>
       <c r="X4" s="1" cm="1">
         <f t="array" ref="X4">IF(
@@ -1607,7 +1614,7 @@
             ROUND((D4 * E4 * PRODUCT(1 - H4:H4 / 100, 1 - L4:L4 / 100, 1 - N4:N4 / 100)), 2)
         ),
     "")</f>
-        <v>10</v>
+        <v>488</v>
       </c>
       <c r="Y4" s="1" t="str" cm="1">
         <f t="array" ref="Y4">IF(
@@ -1673,26 +1680,26 @@
   ),
   2
 )</f>
-        <v>0</v>
+        <v>802.68</v>
       </c>
       <c r="AP4" s="3">
         <f>AK24 / AE3 * (AE3 - AE6)</f>
-        <v>276</v>
+        <v>899</v>
       </c>
       <c r="AQ4" s="3">
         <f>ROUND(AP2 / 1.12 * 0.12, 2)</f>
-        <v>29.57</v>
+        <v>96.32</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>311113</v>
+        <v>35710</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="D5" s="2">
-        <v>29.6</v>
+        <v>488</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1721,16 +1728,13 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>29.6</v>
-      </c>
-      <c r="P5" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="22">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
         <v>0</v>
       </c>
       <c r="S5" s="8" t="str">
@@ -1743,9 +1747,9 @@
       </c>
       <c r="V5" s="33">
         <f t="shared" si="2"/>
-        <v>29.6</v>
-      </c>
-      <c r="X5" s="1" cm="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1" t="str" cm="1">
         <f t="array" ref="X5">IF(
         AND(
             F5=0,
@@ -1757,7 +1761,7 @@
             ROUND((D5 * E5 * PRODUCT(1 - H5:H5 / 100, 1 - L5:L5 / 100, 1 - N5:N5 / 100)), 2)
         ),
     "")</f>
-        <v>29.6</v>
+        <v/>
       </c>
       <c r="Y5" s="1" t="str" cm="1">
         <f t="array" ref="Y5">IF(
@@ -1826,18 +1830,18 @@
       </c>
       <c r="AP5" s="3">
         <f>(AK24)/AE3*(AE3-AE6-AE9-AE12-AE15-AE18-AE21)</f>
-        <v>276</v>
+        <v>899</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>311113</v>
+        <v>35710</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D6" s="2">
-        <v>159.4</v>
+        <v>645</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1866,21 +1870,18 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <v>159.4</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q6" s="22">
+      <c r="O6">
+        <v>645</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
         <v>0</v>
       </c>
       <c r="S6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>VOIDED</v>
+        <v>=</v>
       </c>
       <c r="U6" s="33">
         <f t="shared" si="1"/>
@@ -1888,9 +1889,9 @@
       </c>
       <c r="V6" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="X6" s="1" t="str" cm="1">
+        <v>645</v>
+      </c>
+      <c r="X6" s="1" cm="1">
         <f t="array" ref="X6">IF(
         AND(
             F6=0,
@@ -1902,7 +1903,7 @@
             ROUND((D6 * E6 * PRODUCT(1 - H6:H6 / 100, 1 - L6:L6 / 100, 1 - N6:N6 / 100)), 2)
         ),
     "")</f>
-        <v/>
+        <v>645</v>
       </c>
       <c r="Y6" s="1" t="str" cm="1">
         <f t="array" ref="Y6">IF(
@@ -1961,33 +1962,33 @@
         <v/>
       </c>
       <c r="AE6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6" s="12">
         <v>20</v>
       </c>
       <c r="AK6" s="5">
         <f xml:space="preserve"> (SUM(X:X))</f>
-        <v>276</v>
+        <v>1798</v>
       </c>
       <c r="AO6" s="2">
         <f>ROUND(((AE6=0)*AK18) + ((AE6&lt;&gt;0)*((AK6 + AK9) / AE3 * AE6 / 1.12 + AK18)), 2)</f>
-        <v>0</v>
+        <v>802.68</v>
       </c>
       <c r="AP6" s="3">
         <f>(AK24)/AE3*(AE3-AE6-AE9)</f>
-        <v>276</v>
+        <v>899</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>311113</v>
+        <v>35710</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D7" s="2">
-        <v>159.4</v>
+        <v>645</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2016,16 +2017,13 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
-        <v>159.4</v>
-      </c>
-      <c r="P7" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="22">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
         <v>0</v>
       </c>
       <c r="S7" s="8" t="str">
@@ -2038,9 +2036,9 @@
       </c>
       <c r="V7" s="33">
         <f t="shared" si="2"/>
-        <v>159.4</v>
-      </c>
-      <c r="X7" s="1" cm="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1" t="str" cm="1">
         <f t="array" ref="X7">IF(
         AND(
             F7=0,
@@ -2052,7 +2050,7 @@
             ROUND((D7 * E7 * PRODUCT(1 - H7:H7 / 100, 1 - L7:L7 / 100, 1 - N7:N7 / 100)), 2)
         ),
     "")</f>
-        <v>159.4</v>
+        <v/>
       </c>
       <c r="Y7" s="1" t="str" cm="1">
         <f t="array" ref="Y7">IF(
@@ -2112,6 +2110,51 @@
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>35710</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="2">
+        <v>445</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>445</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
       <c r="S8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -2122,9 +2165,9 @@
       </c>
       <c r="V8" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="X8" s="1" t="str" cm="1">
+        <v>445</v>
+      </c>
+      <c r="X8" s="1" cm="1">
         <f t="array" ref="X8">IF(
         AND(
             F8=0,
@@ -2136,7 +2179,7 @@
             ROUND((D8 * E8 * PRODUCT(1 - H8:H8 / 100, 1 - L8:L8 / 100, 1 - N8:N8 / 100)), 2)
         ),
     "")</f>
-        <v/>
+        <v>445</v>
       </c>
       <c r="Y8" s="1" t="str" cm="1">
         <f t="array" ref="Y8">IF(
@@ -2208,10 +2251,55 @@
      IF((AE6+AE9)=0,
      AK18,
      ((AK6 + AK9) / AE3 *( AE6 + AE9) / 1.12 + AK18)), 2)</f>
-        <v>0</v>
+        <v>802.68</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>35710</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="2">
+        <v>445</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
       <c r="S9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -2307,6 +2395,51 @@
       <c r="AM9" s="3"/>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>35710</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="2">
+        <v>110</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>220</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
       <c r="S10" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -2317,9 +2450,9 @@
       </c>
       <c r="V10" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="X10" s="1" t="str" cm="1">
+        <v>220</v>
+      </c>
+      <c r="X10" s="1" cm="1">
         <f t="array" ref="X10">IF(
         AND(
             F10=0,
@@ -2331,7 +2464,7 @@
             ROUND((D10 * E10 * PRODUCT(1 - H10:H10 / 100, 1 - L10:L10 / 100, 1 - N10:N10 / 100)), 2)
         ),
     "")</f>
-        <v/>
+        <v>220</v>
       </c>
       <c r="Y10" s="1" t="str" cm="1">
         <f t="array" ref="Y10">IF(
@@ -2393,8 +2526,51 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="27"/>
+      <c r="B11">
+        <v>35710</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="27">
+        <v>110</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
       <c r="S11" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -3687,7 +3863,7 @@
       </c>
       <c r="AK24" s="5">
         <f>AK6+AK9</f>
-        <v>276</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -3802,7 +3978,7 @@
         )
     ),
 "Voided")</f>
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -3980,7 +4156,7 @@
       </c>
       <c r="AK27" s="5">
         <f>AK6 / 1.12 * 0.12</f>
-        <v>29.571428571428569</v>
+        <v>192.64285714285711</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -4083,7 +4259,7 @@
         )
     ),
 "Voided")</f>
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -4517,7 +4693,7 @@
       </c>
       <c r="AK33" s="5">
         <f>(((AK3-(AK6/1.12*0.12)) * (AG6*0.01)) / AE3) * AE6</f>
-        <v>0</v>
+        <v>160.53571428571431</v>
       </c>
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.25">
@@ -4605,7 +4781,7 @@
       </c>
       <c r="AK34" s="2">
         <f>(((AK3-(AK24/1.12*0.12)) * (AG6*0.01)) / AE3) * AE6</f>
-        <v>0</v>
+        <v>160.53571428571431</v>
       </c>
     </row>
     <row r="35" spans="1:44" x14ac:dyDescent="0.25">
@@ -4710,9 +4886,9 @@
       <c r="L36"/>
       <c r="M36"/>
       <c r="N36"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
       <c r="S36" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -4828,9 +5004,9 @@
       <c r="L37"/>
       <c r="M37"/>
       <c r="N37"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
       <c r="S37" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -4943,9 +5119,9 @@
       <c r="L38"/>
       <c r="M38"/>
       <c r="N38"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
       <c r="S38" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -5060,9 +5236,9 @@
       <c r="L39"/>
       <c r="M39"/>
       <c r="N39"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="22"/>
-      <c r="Q39" s="22"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
       <c r="S39" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -5153,7 +5329,7 @@
       <c r="AJ39"/>
       <c r="AK39" s="5">
         <f>ROUND(((AE6=0)*AK18) + ((AE6&lt;&gt;0)*((AK6 + AK9) / AE3 * AE6 / 1.12 + AK18)) *0.12, 2)</f>
-        <v>0</v>
+        <v>96.32</v>
       </c>
       <c r="AL39" s="26"/>
       <c r="AM39"/>
@@ -5178,9 +5354,9 @@
       <c r="L40"/>
       <c r="M40"/>
       <c r="N40"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
       <c r="S40" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -5293,9 +5469,9 @@
       <c r="L41"/>
       <c r="M41"/>
       <c r="N41"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="22"/>
-      <c r="Q41" s="22"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
       <c r="S41" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -5410,9 +5586,9 @@
       <c r="L42"/>
       <c r="M42"/>
       <c r="N42"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
       <c r="S42" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -5503,7 +5679,7 @@
       <c r="AJ42"/>
       <c r="AK42" s="5">
         <f xml:space="preserve"> (SUM(X:X)) - (SUM(X:X) / AE3 * AE6)</f>
-        <v>276</v>
+        <v>899</v>
       </c>
       <c r="AL42"/>
       <c r="AM42"/>
@@ -5528,9 +5704,9 @@
       <c r="L43"/>
       <c r="M43"/>
       <c r="N43"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="22"/>
-      <c r="Q43" s="22"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
       <c r="S43" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -5643,9 +5819,9 @@
       <c r="L44"/>
       <c r="M44"/>
       <c r="N44"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
       <c r="S44" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -5760,9 +5936,9 @@
       <c r="L45"/>
       <c r="M45"/>
       <c r="N45"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
       <c r="S45" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -5878,9 +6054,9 @@
       <c r="L46"/>
       <c r="M46"/>
       <c r="N46"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
       <c r="S46" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -5993,9 +6169,9 @@
       <c r="L47"/>
       <c r="M47"/>
       <c r="N47"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="22"/>
-      <c r="Q47" s="22"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
       <c r="S47" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -6110,9 +6286,9 @@
       <c r="L48"/>
       <c r="M48"/>
       <c r="N48"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
       <c r="S48" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -6203,7 +6379,7 @@
       <c r="AJ48"/>
       <c r="AK48" s="5" cm="1">
         <f t="array" ref="AK48">SUMPRODUCT((I2:I1048576&lt;&gt;"") * ((D2:D1048576 * E2:E1048576) - O2:O1048576))</f>
-        <v>0</v>
+        <v>1688</v>
       </c>
       <c r="AL48"/>
       <c r="AM48"/>
@@ -6228,9 +6404,9 @@
       <c r="L49"/>
       <c r="M49"/>
       <c r="N49"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="22"/>
-      <c r="Q49" s="22"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
       <c r="S49" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -6343,9 +6519,9 @@
       <c r="L50"/>
       <c r="M50"/>
       <c r="N50"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
       <c r="S50" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -6434,7 +6610,9 @@
       <c r="AG50"/>
       <c r="AH50"/>
       <c r="AJ50"/>
-      <c r="AK50" s="2"/>
+      <c r="AK50" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="AL50"/>
       <c r="AM50"/>
       <c r="AN50"/>
@@ -6458,9 +6636,9 @@
       <c r="L51"/>
       <c r="M51"/>
       <c r="N51"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
       <c r="S51" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -6549,7 +6727,10 @@
       <c r="AG51"/>
       <c r="AH51"/>
       <c r="AJ51"/>
-      <c r="AK51" s="2"/>
+      <c r="AK51" s="5">
+        <f>(AK6+AK9) / AE3 * AE6 / 1.12 * 0.2</f>
+        <v>160.53571428571428</v>
+      </c>
       <c r="AL51"/>
       <c r="AM51"/>
       <c r="AN51"/>
@@ -6573,9 +6754,9 @@
       <c r="L52"/>
       <c r="M52"/>
       <c r="N52"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="22"/>
-      <c r="Q52" s="22"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
       <c r="S52" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -6688,9 +6869,9 @@
       <c r="L53"/>
       <c r="M53"/>
       <c r="N53"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
       <c r="S53" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -6803,9 +6984,9 @@
       <c r="L54"/>
       <c r="M54"/>
       <c r="N54"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22"/>
+      <c r="O54"/>
+      <c r="P54"/>
+      <c r="Q54"/>
       <c r="S54" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -6918,9 +7099,9 @@
       <c r="L55"/>
       <c r="M55"/>
       <c r="N55"/>
-      <c r="O55" s="2"/>
-      <c r="P55" s="22"/>
-      <c r="Q55" s="22"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
       <c r="S55" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -7033,9 +7214,9 @@
       <c r="L56"/>
       <c r="M56"/>
       <c r="N56"/>
-      <c r="O56" s="2"/>
-      <c r="P56" s="22"/>
-      <c r="Q56" s="22"/>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
       <c r="S56" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -7148,9 +7329,9 @@
       <c r="L57"/>
       <c r="M57"/>
       <c r="N57"/>
-      <c r="O57" s="2"/>
-      <c r="P57" s="22"/>
-      <c r="Q57" s="22"/>
+      <c r="O57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
       <c r="S57" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -7263,9 +7444,9 @@
       <c r="L58"/>
       <c r="M58"/>
       <c r="N58"/>
-      <c r="O58" s="2"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
       <c r="S58" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -7378,9 +7559,9 @@
       <c r="L59"/>
       <c r="M59"/>
       <c r="N59"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="22"/>
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
       <c r="S59" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -7493,9 +7674,9 @@
       <c r="L60"/>
       <c r="M60"/>
       <c r="N60"/>
-      <c r="O60" s="2"/>
-      <c r="P60" s="22"/>
-      <c r="Q60" s="22"/>
+      <c r="O60"/>
+      <c r="P60"/>
+      <c r="Q60"/>
       <c r="S60" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -7608,9 +7789,9 @@
       <c r="L61"/>
       <c r="M61"/>
       <c r="N61"/>
-      <c r="O61" s="2"/>
-      <c r="P61" s="22"/>
-      <c r="Q61" s="22"/>
+      <c r="O61"/>
+      <c r="P61"/>
+      <c r="Q61"/>
       <c r="S61" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -7723,9 +7904,9 @@
       <c r="L62"/>
       <c r="M62"/>
       <c r="N62"/>
-      <c r="O62" s="2"/>
-      <c r="P62" s="22"/>
-      <c r="Q62" s="22"/>
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
       <c r="S62" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -7838,9 +8019,9 @@
       <c r="L63"/>
       <c r="M63"/>
       <c r="N63"/>
-      <c r="O63" s="2"/>
-      <c r="P63" s="22"/>
-      <c r="Q63" s="22"/>
+      <c r="O63"/>
+      <c r="P63"/>
+      <c r="Q63"/>
       <c r="S63" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -7953,9 +8134,9 @@
       <c r="L64"/>
       <c r="M64"/>
       <c r="N64"/>
-      <c r="O64" s="2"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="22"/>
+      <c r="O64"/>
+      <c r="P64"/>
+      <c r="Q64"/>
       <c r="S64" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -8068,9 +8249,9 @@
       <c r="L65"/>
       <c r="M65"/>
       <c r="N65"/>
-      <c r="O65" s="2"/>
-      <c r="P65" s="22"/>
-      <c r="Q65" s="22"/>
+      <c r="O65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
       <c r="S65" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -8183,9 +8364,9 @@
       <c r="L66"/>
       <c r="M66"/>
       <c r="N66"/>
-      <c r="O66" s="2"/>
-      <c r="P66" s="22"/>
-      <c r="Q66" s="22"/>
+      <c r="O66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
       <c r="S66" s="8" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
@@ -8298,9 +8479,9 @@
       <c r="L67"/>
       <c r="M67"/>
       <c r="N67"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="22"/>
-      <c r="Q67" s="22"/>
+      <c r="O67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
       <c r="S67" s="8" t="str">
         <f t="shared" ref="S67:S130" si="3">IF(OR(P67=0,P67=1),
 IF(AND(O67=V67, Q67=U67), "=","NOT EQUAL"), "VOIDED")</f>
@@ -8308,7 +8489,10 @@
       </c>
       <c r="U67" s="33">
         <f t="shared" ref="U67:U130" si="4">IF(
-            OR(P67=0, P67=1),
+            AND(
+                OR(P67=0, P67=1),
+                O67&lt;&gt;0
+            ),
             IF(G67&gt;0,
                 Q67,
                 IF(
@@ -8330,7 +8514,10 @@
       </c>
       <c r="V67" s="33">
         <f t="shared" ref="V67:V130" si="5">IF(
-            OR(P67=0, P67=1),
+            AND(
+                OR(P67=0, P67=1),
+                O67&lt;&gt;0
+            ),
             IF(
                 OR(G67&gt;0, H67&gt;0),
                 D67 * E67 - IF(G67&gt;0, Q67, D67 * E67 * H67 / 100),
@@ -8463,9 +8650,9 @@
       <c r="L68"/>
       <c r="M68"/>
       <c r="N68"/>
-      <c r="O68" s="2"/>
-      <c r="P68" s="22"/>
-      <c r="Q68" s="22"/>
+      <c r="O68"/>
+      <c r="P68"/>
+      <c r="Q68"/>
       <c r="S68" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -8578,9 +8765,9 @@
       <c r="L69"/>
       <c r="M69"/>
       <c r="N69"/>
-      <c r="O69" s="2"/>
-      <c r="P69" s="22"/>
-      <c r="Q69" s="22"/>
+      <c r="O69"/>
+      <c r="P69"/>
+      <c r="Q69"/>
       <c r="S69" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -8693,9 +8880,9 @@
       <c r="L70"/>
       <c r="M70"/>
       <c r="N70"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="22"/>
-      <c r="Q70" s="22"/>
+      <c r="O70"/>
+      <c r="P70"/>
+      <c r="Q70"/>
       <c r="S70" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -8808,9 +8995,9 @@
       <c r="L71"/>
       <c r="M71"/>
       <c r="N71"/>
-      <c r="O71" s="2"/>
-      <c r="P71" s="22"/>
-      <c r="Q71" s="22"/>
+      <c r="O71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
       <c r="S71" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -8923,9 +9110,9 @@
       <c r="L72"/>
       <c r="M72"/>
       <c r="N72"/>
-      <c r="O72" s="2"/>
-      <c r="P72" s="22"/>
-      <c r="Q72" s="22"/>
+      <c r="O72"/>
+      <c r="P72"/>
+      <c r="Q72"/>
       <c r="S72" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -9038,9 +9225,9 @@
       <c r="L73"/>
       <c r="M73"/>
       <c r="N73"/>
-      <c r="O73" s="2"/>
-      <c r="P73" s="22"/>
-      <c r="Q73" s="22"/>
+      <c r="O73"/>
+      <c r="P73"/>
+      <c r="Q73"/>
       <c r="S73" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -9153,9 +9340,9 @@
       <c r="L74"/>
       <c r="M74"/>
       <c r="N74"/>
-      <c r="O74" s="2"/>
-      <c r="P74" s="22"/>
-      <c r="Q74" s="22"/>
+      <c r="O74"/>
+      <c r="P74"/>
+      <c r="Q74"/>
       <c r="S74" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -9268,9 +9455,9 @@
       <c r="L75"/>
       <c r="M75"/>
       <c r="N75"/>
-      <c r="O75" s="2"/>
-      <c r="P75" s="22"/>
-      <c r="Q75" s="22"/>
+      <c r="O75"/>
+      <c r="P75"/>
+      <c r="Q75"/>
       <c r="S75" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -9383,9 +9570,9 @@
       <c r="L76"/>
       <c r="M76"/>
       <c r="N76"/>
-      <c r="O76" s="2"/>
-      <c r="P76" s="22"/>
-      <c r="Q76" s="22"/>
+      <c r="O76"/>
+      <c r="P76"/>
+      <c r="Q76"/>
       <c r="S76" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -9498,9 +9685,9 @@
       <c r="L77"/>
       <c r="M77"/>
       <c r="N77"/>
-      <c r="O77" s="2"/>
-      <c r="P77" s="22"/>
-      <c r="Q77" s="22"/>
+      <c r="O77"/>
+      <c r="P77"/>
+      <c r="Q77"/>
       <c r="S77" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -9613,9 +9800,9 @@
       <c r="L78"/>
       <c r="M78"/>
       <c r="N78"/>
-      <c r="O78" s="2"/>
-      <c r="P78" s="22"/>
-      <c r="Q78" s="22"/>
+      <c r="O78"/>
+      <c r="P78"/>
+      <c r="Q78"/>
       <c r="S78" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -9728,9 +9915,9 @@
       <c r="L79"/>
       <c r="M79"/>
       <c r="N79"/>
-      <c r="O79" s="2"/>
-      <c r="P79" s="22"/>
-      <c r="Q79" s="22"/>
+      <c r="O79"/>
+      <c r="P79"/>
+      <c r="Q79"/>
       <c r="S79" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -9843,9 +10030,9 @@
       <c r="L80"/>
       <c r="M80"/>
       <c r="N80"/>
-      <c r="O80" s="2"/>
-      <c r="P80" s="22"/>
-      <c r="Q80" s="22"/>
+      <c r="O80"/>
+      <c r="P80"/>
+      <c r="Q80"/>
       <c r="S80" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -9958,9 +10145,9 @@
       <c r="L81"/>
       <c r="M81"/>
       <c r="N81"/>
-      <c r="O81" s="2"/>
-      <c r="P81" s="22"/>
-      <c r="Q81" s="22"/>
+      <c r="O81"/>
+      <c r="P81"/>
+      <c r="Q81"/>
       <c r="S81" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -10073,9 +10260,9 @@
       <c r="L82"/>
       <c r="M82"/>
       <c r="N82"/>
-      <c r="O82" s="2"/>
-      <c r="P82" s="22"/>
-      <c r="Q82" s="22"/>
+      <c r="O82"/>
+      <c r="P82"/>
+      <c r="Q82"/>
       <c r="S82" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -10188,9 +10375,9 @@
       <c r="L83"/>
       <c r="M83"/>
       <c r="N83"/>
-      <c r="O83" s="2"/>
-      <c r="P83" s="22"/>
-      <c r="Q83" s="22"/>
+      <c r="O83"/>
+      <c r="P83"/>
+      <c r="Q83"/>
       <c r="S83" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -10303,9 +10490,9 @@
       <c r="L84"/>
       <c r="M84"/>
       <c r="N84"/>
-      <c r="O84" s="2"/>
-      <c r="P84" s="22"/>
-      <c r="Q84" s="22"/>
+      <c r="O84"/>
+      <c r="P84"/>
+      <c r="Q84"/>
       <c r="S84" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -10418,9 +10605,9 @@
       <c r="L85"/>
       <c r="M85"/>
       <c r="N85"/>
-      <c r="O85" s="2"/>
-      <c r="P85" s="22"/>
-      <c r="Q85" s="22"/>
+      <c r="O85"/>
+      <c r="P85"/>
+      <c r="Q85"/>
       <c r="S85" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -10533,9 +10720,9 @@
       <c r="L86"/>
       <c r="M86"/>
       <c r="N86"/>
-      <c r="O86" s="2"/>
-      <c r="P86" s="22"/>
-      <c r="Q86" s="22"/>
+      <c r="O86"/>
+      <c r="P86"/>
+      <c r="Q86"/>
       <c r="S86" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -10648,9 +10835,9 @@
       <c r="L87"/>
       <c r="M87"/>
       <c r="N87"/>
-      <c r="O87" s="2"/>
-      <c r="P87" s="22"/>
-      <c r="Q87" s="22"/>
+      <c r="O87"/>
+      <c r="P87"/>
+      <c r="Q87"/>
       <c r="S87" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -10763,9 +10950,9 @@
       <c r="L88"/>
       <c r="M88"/>
       <c r="N88"/>
-      <c r="O88" s="2"/>
-      <c r="P88" s="22"/>
-      <c r="Q88" s="22"/>
+      <c r="O88"/>
+      <c r="P88"/>
+      <c r="Q88"/>
       <c r="S88" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -10878,9 +11065,9 @@
       <c r="L89"/>
       <c r="M89"/>
       <c r="N89"/>
-      <c r="O89" s="2"/>
-      <c r="P89" s="22"/>
-      <c r="Q89" s="22"/>
+      <c r="O89"/>
+      <c r="P89"/>
+      <c r="Q89"/>
       <c r="S89" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -10993,9 +11180,9 @@
       <c r="L90"/>
       <c r="M90"/>
       <c r="N90"/>
-      <c r="O90" s="2"/>
-      <c r="P90" s="22"/>
-      <c r="Q90" s="22"/>
+      <c r="O90"/>
+      <c r="P90"/>
+      <c r="Q90"/>
       <c r="S90" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -11108,9 +11295,9 @@
       <c r="L91"/>
       <c r="M91"/>
       <c r="N91"/>
-      <c r="O91" s="2"/>
-      <c r="P91" s="22"/>
-      <c r="Q91" s="22"/>
+      <c r="O91"/>
+      <c r="P91"/>
+      <c r="Q91"/>
       <c r="S91" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -11223,9 +11410,9 @@
       <c r="L92"/>
       <c r="M92"/>
       <c r="N92"/>
-      <c r="O92" s="2"/>
-      <c r="P92" s="22"/>
-      <c r="Q92" s="22"/>
+      <c r="O92"/>
+      <c r="P92"/>
+      <c r="Q92"/>
       <c r="S92" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -11338,9 +11525,9 @@
       <c r="L93"/>
       <c r="M93"/>
       <c r="N93"/>
-      <c r="O93" s="2"/>
-      <c r="P93" s="22"/>
-      <c r="Q93" s="22"/>
+      <c r="O93"/>
+      <c r="P93"/>
+      <c r="Q93"/>
       <c r="S93" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -11453,9 +11640,9 @@
       <c r="L94"/>
       <c r="M94"/>
       <c r="N94"/>
-      <c r="O94" s="2"/>
-      <c r="P94" s="22"/>
-      <c r="Q94" s="22"/>
+      <c r="O94"/>
+      <c r="P94"/>
+      <c r="Q94"/>
       <c r="S94" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -11568,9 +11755,9 @@
       <c r="L95"/>
       <c r="M95"/>
       <c r="N95"/>
-      <c r="O95" s="2"/>
-      <c r="P95" s="22"/>
-      <c r="Q95" s="22"/>
+      <c r="O95"/>
+      <c r="P95"/>
+      <c r="Q95"/>
       <c r="S95" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -11683,9 +11870,9 @@
       <c r="L96"/>
       <c r="M96"/>
       <c r="N96"/>
-      <c r="O96" s="2"/>
-      <c r="P96" s="22"/>
-      <c r="Q96" s="22"/>
+      <c r="O96"/>
+      <c r="P96"/>
+      <c r="Q96"/>
       <c r="S96" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -11798,9 +11985,9 @@
       <c r="L97"/>
       <c r="M97"/>
       <c r="N97"/>
-      <c r="O97" s="2"/>
-      <c r="P97" s="22"/>
-      <c r="Q97" s="22"/>
+      <c r="O97"/>
+      <c r="P97"/>
+      <c r="Q97"/>
       <c r="S97" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -11913,9 +12100,9 @@
       <c r="L98"/>
       <c r="M98"/>
       <c r="N98"/>
-      <c r="O98" s="2"/>
-      <c r="P98" s="22"/>
-      <c r="Q98" s="22"/>
+      <c r="O98"/>
+      <c r="P98"/>
+      <c r="Q98"/>
       <c r="S98" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -12028,9 +12215,9 @@
       <c r="L99"/>
       <c r="M99"/>
       <c r="N99"/>
-      <c r="O99" s="2"/>
-      <c r="P99" s="22"/>
-      <c r="Q99" s="22"/>
+      <c r="O99"/>
+      <c r="P99"/>
+      <c r="Q99"/>
       <c r="S99" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -12143,9 +12330,9 @@
       <c r="L100"/>
       <c r="M100"/>
       <c r="N100"/>
-      <c r="O100" s="2"/>
-      <c r="P100" s="22"/>
-      <c r="Q100" s="22"/>
+      <c r="O100"/>
+      <c r="P100"/>
+      <c r="Q100"/>
       <c r="S100" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -12258,9 +12445,9 @@
       <c r="L101"/>
       <c r="M101"/>
       <c r="N101"/>
-      <c r="O101" s="2"/>
-      <c r="P101" s="22"/>
-      <c r="Q101" s="22"/>
+      <c r="O101"/>
+      <c r="P101"/>
+      <c r="Q101"/>
       <c r="S101" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -12373,9 +12560,9 @@
       <c r="L102"/>
       <c r="M102"/>
       <c r="N102"/>
-      <c r="O102" s="2"/>
-      <c r="P102" s="22"/>
-      <c r="Q102" s="22"/>
+      <c r="O102"/>
+      <c r="P102"/>
+      <c r="Q102"/>
       <c r="S102" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -12488,9 +12675,9 @@
       <c r="L103"/>
       <c r="M103"/>
       <c r="N103"/>
-      <c r="O103" s="2"/>
-      <c r="P103" s="22"/>
-      <c r="Q103" s="22"/>
+      <c r="O103"/>
+      <c r="P103"/>
+      <c r="Q103"/>
       <c r="S103" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -12603,9 +12790,9 @@
       <c r="L104"/>
       <c r="M104"/>
       <c r="N104"/>
-      <c r="O104" s="2"/>
-      <c r="P104" s="22"/>
-      <c r="Q104" s="22"/>
+      <c r="O104"/>
+      <c r="P104"/>
+      <c r="Q104"/>
       <c r="S104" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -12718,9 +12905,9 @@
       <c r="L105"/>
       <c r="M105"/>
       <c r="N105"/>
-      <c r="O105" s="2"/>
-      <c r="P105" s="22"/>
-      <c r="Q105" s="22"/>
+      <c r="O105"/>
+      <c r="P105"/>
+      <c r="Q105"/>
       <c r="S105" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -12833,9 +13020,9 @@
       <c r="L106"/>
       <c r="M106"/>
       <c r="N106"/>
-      <c r="O106" s="2"/>
-      <c r="P106" s="22"/>
-      <c r="Q106" s="22"/>
+      <c r="O106"/>
+      <c r="P106"/>
+      <c r="Q106"/>
       <c r="S106" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -12948,9 +13135,9 @@
       <c r="L107"/>
       <c r="M107"/>
       <c r="N107"/>
-      <c r="O107" s="2"/>
-      <c r="P107" s="22"/>
-      <c r="Q107" s="22"/>
+      <c r="O107"/>
+      <c r="P107"/>
+      <c r="Q107"/>
       <c r="S107" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -13063,9 +13250,9 @@
       <c r="L108"/>
       <c r="M108"/>
       <c r="N108"/>
-      <c r="O108" s="2"/>
-      <c r="P108" s="22"/>
-      <c r="Q108" s="22"/>
+      <c r="O108"/>
+      <c r="P108"/>
+      <c r="Q108"/>
       <c r="S108" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -13178,9 +13365,9 @@
       <c r="L109"/>
       <c r="M109"/>
       <c r="N109"/>
-      <c r="O109" s="2"/>
-      <c r="P109" s="22"/>
-      <c r="Q109" s="22"/>
+      <c r="O109"/>
+      <c r="P109"/>
+      <c r="Q109"/>
       <c r="S109" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -13293,9 +13480,9 @@
       <c r="L110"/>
       <c r="M110"/>
       <c r="N110"/>
-      <c r="O110" s="2"/>
-      <c r="P110" s="22"/>
-      <c r="Q110" s="22"/>
+      <c r="O110"/>
+      <c r="P110"/>
+      <c r="Q110"/>
       <c r="S110" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -13408,9 +13595,9 @@
       <c r="L111"/>
       <c r="M111"/>
       <c r="N111"/>
-      <c r="O111" s="2"/>
-      <c r="P111" s="22"/>
-      <c r="Q111" s="22"/>
+      <c r="O111"/>
+      <c r="P111"/>
+      <c r="Q111"/>
       <c r="S111" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -13523,9 +13710,9 @@
       <c r="L112"/>
       <c r="M112"/>
       <c r="N112"/>
-      <c r="O112" s="2"/>
-      <c r="P112" s="22"/>
-      <c r="Q112" s="22"/>
+      <c r="O112"/>
+      <c r="P112"/>
+      <c r="Q112"/>
       <c r="S112" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -13638,9 +13825,9 @@
       <c r="L113"/>
       <c r="M113"/>
       <c r="N113"/>
-      <c r="O113" s="2"/>
-      <c r="P113" s="22"/>
-      <c r="Q113" s="22"/>
+      <c r="O113"/>
+      <c r="P113"/>
+      <c r="Q113"/>
       <c r="S113" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -13753,9 +13940,9 @@
       <c r="L114"/>
       <c r="M114"/>
       <c r="N114"/>
-      <c r="O114" s="2"/>
-      <c r="P114" s="22"/>
-      <c r="Q114" s="22"/>
+      <c r="O114"/>
+      <c r="P114"/>
+      <c r="Q114"/>
       <c r="S114" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -13868,9 +14055,9 @@
       <c r="L115"/>
       <c r="M115"/>
       <c r="N115"/>
-      <c r="O115" s="2"/>
-      <c r="P115" s="22"/>
-      <c r="Q115" s="22"/>
+      <c r="O115"/>
+      <c r="P115"/>
+      <c r="Q115"/>
       <c r="S115" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -13983,9 +14170,9 @@
       <c r="L116"/>
       <c r="M116"/>
       <c r="N116"/>
-      <c r="O116" s="2"/>
-      <c r="P116" s="22"/>
-      <c r="Q116" s="22"/>
+      <c r="O116"/>
+      <c r="P116"/>
+      <c r="Q116"/>
       <c r="S116" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -14098,9 +14285,9 @@
       <c r="L117"/>
       <c r="M117"/>
       <c r="N117"/>
-      <c r="O117" s="2"/>
-      <c r="P117" s="22"/>
-      <c r="Q117" s="22"/>
+      <c r="O117"/>
+      <c r="P117"/>
+      <c r="Q117"/>
       <c r="S117" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -14213,9 +14400,9 @@
       <c r="L118"/>
       <c r="M118"/>
       <c r="N118"/>
-      <c r="O118" s="2"/>
-      <c r="P118" s="22"/>
-      <c r="Q118" s="22"/>
+      <c r="O118"/>
+      <c r="P118"/>
+      <c r="Q118"/>
       <c r="S118" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -14328,9 +14515,9 @@
       <c r="L119"/>
       <c r="M119"/>
       <c r="N119"/>
-      <c r="O119" s="2"/>
-      <c r="P119" s="22"/>
-      <c r="Q119" s="22"/>
+      <c r="O119"/>
+      <c r="P119"/>
+      <c r="Q119"/>
       <c r="S119" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -14443,9 +14630,9 @@
       <c r="L120"/>
       <c r="M120"/>
       <c r="N120"/>
-      <c r="O120" s="2"/>
-      <c r="P120" s="22"/>
-      <c r="Q120" s="22"/>
+      <c r="O120"/>
+      <c r="P120"/>
+      <c r="Q120"/>
       <c r="S120" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -14558,9 +14745,9 @@
       <c r="L121"/>
       <c r="M121"/>
       <c r="N121"/>
-      <c r="O121" s="2"/>
-      <c r="P121" s="22"/>
-      <c r="Q121" s="22"/>
+      <c r="O121"/>
+      <c r="P121"/>
+      <c r="Q121"/>
       <c r="S121" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -14673,9 +14860,9 @@
       <c r="L122"/>
       <c r="M122"/>
       <c r="N122"/>
-      <c r="O122" s="2"/>
-      <c r="P122" s="22"/>
-      <c r="Q122" s="22"/>
+      <c r="O122"/>
+      <c r="P122"/>
+      <c r="Q122"/>
       <c r="S122" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -14788,9 +14975,9 @@
       <c r="L123"/>
       <c r="M123"/>
       <c r="N123"/>
-      <c r="O123" s="2"/>
-      <c r="P123" s="22"/>
-      <c r="Q123" s="22"/>
+      <c r="O123"/>
+      <c r="P123"/>
+      <c r="Q123"/>
       <c r="S123" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -14903,9 +15090,9 @@
       <c r="L124"/>
       <c r="M124"/>
       <c r="N124"/>
-      <c r="O124" s="2"/>
-      <c r="P124" s="22"/>
-      <c r="Q124" s="22"/>
+      <c r="O124"/>
+      <c r="P124"/>
+      <c r="Q124"/>
       <c r="S124" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -15018,9 +15205,9 @@
       <c r="L125"/>
       <c r="M125"/>
       <c r="N125"/>
-      <c r="O125" s="2"/>
-      <c r="P125" s="22"/>
-      <c r="Q125" s="22"/>
+      <c r="O125"/>
+      <c r="P125"/>
+      <c r="Q125"/>
       <c r="S125" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -15133,9 +15320,9 @@
       <c r="L126"/>
       <c r="M126"/>
       <c r="N126"/>
-      <c r="O126" s="2"/>
-      <c r="P126" s="22"/>
-      <c r="Q126" s="22"/>
+      <c r="O126"/>
+      <c r="P126"/>
+      <c r="Q126"/>
       <c r="S126" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -15248,9 +15435,9 @@
       <c r="L127"/>
       <c r="M127"/>
       <c r="N127"/>
-      <c r="O127" s="2"/>
-      <c r="P127" s="22"/>
-      <c r="Q127" s="22"/>
+      <c r="O127"/>
+      <c r="P127"/>
+      <c r="Q127"/>
       <c r="S127" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -15363,9 +15550,9 @@
       <c r="L128"/>
       <c r="M128"/>
       <c r="N128"/>
-      <c r="O128" s="2"/>
-      <c r="P128" s="22"/>
-      <c r="Q128" s="22"/>
+      <c r="O128"/>
+      <c r="P128"/>
+      <c r="Q128"/>
       <c r="S128" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -15478,9 +15665,9 @@
       <c r="L129"/>
       <c r="M129"/>
       <c r="N129"/>
-      <c r="O129" s="2"/>
-      <c r="P129" s="22"/>
-      <c r="Q129" s="22"/>
+      <c r="O129"/>
+      <c r="P129"/>
+      <c r="Q129"/>
       <c r="S129" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -15593,9 +15780,9 @@
       <c r="L130"/>
       <c r="M130"/>
       <c r="N130"/>
-      <c r="O130" s="2"/>
-      <c r="P130" s="22"/>
-      <c r="Q130" s="22"/>
+      <c r="O130"/>
+      <c r="P130"/>
+      <c r="Q130"/>
       <c r="S130" s="8" t="str">
         <f t="shared" si="3"/>
         <v>=</v>
@@ -15708,9 +15895,9 @@
       <c r="L131"/>
       <c r="M131"/>
       <c r="N131"/>
-      <c r="O131" s="2"/>
-      <c r="P131" s="22"/>
-      <c r="Q131" s="22"/>
+      <c r="O131"/>
+      <c r="P131"/>
+      <c r="Q131"/>
       <c r="S131" s="8" t="str">
         <f t="shared" ref="S131:S134" si="6">IF(OR(P131=0,P131=1),
 IF(AND(O131=V131, Q131=U131), "=","NOT EQUAL"), "VOIDED")</f>
@@ -15718,7 +15905,10 @@
       </c>
       <c r="U131" s="33">
         <f t="shared" ref="U131:U134" si="7">IF(
-            OR(P131=0, P131=1),
+            AND(
+                OR(P131=0, P131=1),
+                O131&lt;&gt;0
+            ),
             IF(G131&gt;0,
                 Q131,
                 IF(
@@ -15740,7 +15930,10 @@
       </c>
       <c r="V131" s="33">
         <f t="shared" ref="V131:V134" si="8">IF(
-            OR(P131=0, P131=1),
+            AND(
+                OR(P131=0, P131=1),
+                O131&lt;&gt;0
+            ),
             IF(
                 OR(G131&gt;0, H131&gt;0),
                 D131 * E131 - IF(G131&gt;0, Q131, D131 * E131 * H131 / 100),
@@ -15873,9 +16066,9 @@
       <c r="L132"/>
       <c r="M132"/>
       <c r="N132"/>
-      <c r="O132" s="2"/>
-      <c r="P132" s="22"/>
-      <c r="Q132" s="22"/>
+      <c r="O132"/>
+      <c r="P132"/>
+      <c r="Q132"/>
       <c r="S132" s="8" t="str">
         <f t="shared" si="6"/>
         <v>=</v>
@@ -15988,9 +16181,9 @@
       <c r="L133"/>
       <c r="M133"/>
       <c r="N133"/>
-      <c r="O133" s="2"/>
-      <c r="P133" s="22"/>
-      <c r="Q133" s="22"/>
+      <c r="O133"/>
+      <c r="P133"/>
+      <c r="Q133"/>
       <c r="S133" s="8" t="str">
         <f t="shared" si="6"/>
         <v>=</v>
@@ -16103,9 +16296,9 @@
       <c r="L134"/>
       <c r="M134"/>
       <c r="N134"/>
-      <c r="O134" s="2"/>
-      <c r="P134" s="22"/>
-      <c r="Q134" s="22"/>
+      <c r="O134"/>
+      <c r="P134"/>
+      <c r="Q134"/>
       <c r="S134" s="8" t="str">
         <f t="shared" si="6"/>
         <v>=</v>
@@ -16270,10 +16463,10 @@
         <v>6</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R1" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S1" s="13" t="s">
         <v>56</v>
@@ -16323,10 +16516,10 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R2" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S2" s="13" t="s">
         <v>0</v>
@@ -16376,10 +16569,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R3" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S3" s="13" t="s">
         <v>1</v>
@@ -16429,10 +16622,10 @@
         <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R4" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S4" s="14" t="s">
         <v>3</v>
@@ -16482,10 +16675,10 @@
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R5" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S5" s="13" t="s">
         <v>2</v>
@@ -16493,10 +16686,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="R6" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S6" s="13" t="s">
         <v>4</v>
@@ -16513,7 +16706,7 @@
         <v>85</v>
       </c>
       <c r="R7" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S7" s="13" t="s">
         <v>69</v>
@@ -16530,7 +16723,7 @@
         <v>70</v>
       </c>
       <c r="R8" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S8" s="13" t="s">
         <v>51</v>
@@ -16547,7 +16740,7 @@
         <v>71</v>
       </c>
       <c r="R9" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S9" s="13" t="s">
         <v>7</v>
@@ -16564,7 +16757,7 @@
         <v>72</v>
       </c>
       <c r="R10" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S10" s="13" t="s">
         <v>52</v>
@@ -16581,7 +16774,7 @@
         <v>73</v>
       </c>
       <c r="R11" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S11" s="13" t="s">
         <v>53</v>
@@ -16598,7 +16791,7 @@
         <v>74</v>
       </c>
       <c r="R12" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S12" s="13" t="s">
         <v>54</v>
@@ -16615,7 +16808,7 @@
         <v>75</v>
       </c>
       <c r="R13" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S13" s="13" t="s">
         <v>55</v>
@@ -16632,7 +16825,7 @@
         <v>76</v>
       </c>
       <c r="R14" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S14" s="13" t="s">
         <v>57</v>
@@ -16640,10 +16833,10 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R15" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S15" s="14" t="s">
         <v>5</v>
@@ -16651,10 +16844,10 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R16" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S16" s="13" t="s">
         <v>6</v>
@@ -16662,10 +16855,10 @@
     </row>
     <row r="17" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R17" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S17" s="13" t="s">
         <v>86</v>
@@ -16673,37 +16866,37 @@
     </row>
     <row r="18" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="R18" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R19" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S19" s="8"/>
     </row>
     <row r="20" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R20" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S20" s="10"/>
     </row>
     <row r="21" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R21" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S21" s="9" t="s">
         <v>87</v>
@@ -16711,10 +16904,10 @@
     </row>
     <row r="22" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R22" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S22" s="9" t="s">
         <v>13</v>
@@ -16722,19 +16915,19 @@
     </row>
     <row r="23" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R23" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S23" s="10"/>
     </row>
     <row r="24" spans="17:19" ht="30" x14ac:dyDescent="0.25">
       <c r="Q24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R24" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S24" s="17" t="s">
         <v>19</v>
@@ -16742,10 +16935,10 @@
     </row>
     <row r="25" spans="17:19" ht="30" x14ac:dyDescent="0.25">
       <c r="Q25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="R25" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S25" s="17" t="s">
         <v>20</v>
@@ -16753,10 +16946,10 @@
     </row>
     <row r="26" spans="17:19" ht="30" x14ac:dyDescent="0.25">
       <c r="Q26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="R26" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S26" s="17" t="s">
         <v>21</v>
@@ -16764,10 +16957,10 @@
     </row>
     <row r="27" spans="17:19" ht="30" x14ac:dyDescent="0.25">
       <c r="Q27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="R27" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S27" s="17" t="s">
         <v>22</v>
@@ -16775,10 +16968,10 @@
     </row>
     <row r="28" spans="17:19" ht="30" x14ac:dyDescent="0.25">
       <c r="Q28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R28" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S28" s="17" t="s">
         <v>18</v>
@@ -16786,28 +16979,28 @@
     </row>
     <row r="29" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="R29" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S29" s="10"/>
     </row>
     <row r="30" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R30" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="R31" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S31" s="8" t="s">
         <v>10</v>
@@ -16815,19 +17008,19 @@
     </row>
     <row r="32" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R32" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S32" s="8"/>
     </row>
     <row r="33" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="R33" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S33" s="8" t="s">
         <v>30</v>
@@ -16835,37 +17028,37 @@
     </row>
     <row r="34" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="R34" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="R35" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S35" s="10"/>
     </row>
     <row r="36" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R36" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R37" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S37" s="9" t="s">
         <v>9</v>
@@ -16873,19 +17066,19 @@
     </row>
     <row r="38" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R38" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S38" s="20"/>
     </row>
     <row r="39" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R39" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S39" s="11" t="s">
         <v>12</v>
@@ -16893,10 +17086,10 @@
     </row>
     <row r="40" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="R40" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S40" s="10" t="s">
         <v>17</v>
@@ -16904,10 +17097,10 @@
     </row>
     <row r="41" spans="17:19" ht="30" x14ac:dyDescent="0.25">
       <c r="Q41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R41" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S41" s="23" t="s">
         <v>14</v>
@@ -16915,10 +17108,10 @@
     </row>
     <row r="42" spans="17:19" ht="30" x14ac:dyDescent="0.25">
       <c r="Q42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="R42" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S42" s="15" t="s">
         <v>15</v>
@@ -16926,10 +17119,10 @@
     </row>
     <row r="43" spans="17:19" ht="30" x14ac:dyDescent="0.25">
       <c r="Q43" t="s">
+        <v>121</v>
+      </c>
+      <c r="R43" s="34" t="s">
         <v>123</v>
-      </c>
-      <c r="R43" s="34" t="s">
-        <v>125</v>
       </c>
       <c r="S43" s="21" t="s">
         <v>16</v>

</xml_diff>